<commit_message>
report results and PPT
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palmo\OneDrive\Documents\GitHub\SEcube'structure'branch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE7FC0DD-1ED6-4A36-850C-2FB20C41AD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3FB5F6-9B63-4C52-AAC5-80E0CB0591BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{18760C7E-6D15-4877-B866-7E3134B17E7A}"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="17304" windowHeight="8892" xr2:uid="{18760C7E-6D15-4877-B866-7E3134B17E7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -235,37 +235,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1655,7 +1625,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>